<commit_message>
Nenávidím tenhle předmĚt já chci spát prosím
</commit_message>
<xml_diff>
--- a/Uloha3/Kopie - impedance - otevreny natrubek 2.xlsx
+++ b/Uloha3/Kopie - impedance - otevreny natrubek 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vutbr-my.sharepoint.com/personal/247759_vutbr_cz/Documents/Bc. 5. Semestr/BPC-MVAA/BPC-MVAA-Protokoly-2024/Uloha3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCDE2C4D-35E8-4F7E-AC58-B8E6A1194FFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{CCDE2C4D-35E8-4F7E-AC58-B8E6A1194FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF1BA0DE-6B2E-472C-98B7-963045BBAB7D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31812" yWindow="360" windowWidth="30720" windowHeight="16272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mereni" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,21 @@
   <definedNames>
     <definedName name="pokus">Mereni!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -488,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -500,7 +511,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -509,16 +520,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -527,9 +538,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -547,7 +559,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="cs-CZ"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2700,22 +2712,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="18.7109375" customWidth="1"/>
+    <col min="1" max="6" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2735,7 +2749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -2755,7 +2769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>20</v>
       </c>
@@ -2775,7 +2789,7 @@
         <v>17.231944169054</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>30</v>
       </c>
@@ -2795,7 +2809,7 @@
         <v>21.867329977353702</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>35</v>
       </c>
@@ -2815,7 +2829,7 @@
         <v>30.481863677356099</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>37</v>
       </c>
@@ -2835,7 +2849,7 @@
         <v>29.318733299654902</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>40</v>
       </c>
@@ -2855,7 +2869,7 @@
         <v>16.476494661037002</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>43</v>
       </c>
@@ -2875,7 +2889,7 @@
         <v>13.297749680739299</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>45</v>
       </c>
@@ -2895,7 +2909,7 @@
         <v>16.175528399834999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>50</v>
       </c>
@@ -2915,7 +2929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>60</v>
       </c>
@@ -2935,7 +2949,7 @@
         <v>6.0867078384416203E-7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>65</v>
       </c>
@@ -2955,7 +2969,7 @@
         <v>13.6817086899177</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>70</v>
       </c>
@@ -2975,7 +2989,7 @@
         <v>21.032270538553998</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>75</v>
       </c>
@@ -2995,7 +3009,7 @@
         <v>20.7605726348893</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>80</v>
       </c>
@@ -3015,7 +3029,7 @@
         <v>29.5775867760998</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>90</v>
       </c>
@@ -3035,7 +3049,7 @@
         <v>34.470519644257898</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>100</v>
       </c>
@@ -3055,7 +3069,7 @@
         <v>41.780235857114697</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>110</v>
       </c>
@@ -3075,7 +3089,7 @@
         <v>40.922239605999998</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>115</v>
       </c>
@@ -3095,7 +3109,7 @@
         <v>26.816389798671</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>120</v>
       </c>
@@ -3115,7 +3129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <v>125</v>
       </c>
@@ -3135,7 +3149,7 @@
         <v>28.954866773655599</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>130</v>
       </c>
@@ -3155,7 +3169,7 @@
         <v>35.156900837041803</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <v>140</v>
       </c>
@@ -3175,7 +3189,7 @@
         <v>38.625279310827899</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>160</v>
       </c>
@@ -3195,7 +3209,7 @@
         <v>26.577405531896499</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <v>180</v>
       </c>
@@ -3215,7 +3229,7 @@
         <v>17.021527886003401</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <v>200</v>
       </c>
@@ -3235,7 +3249,7 @@
         <v>12.2510693499684</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>300</v>
       </c>
@@ -3255,7 +3269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <v>400</v>
       </c>
@@ -3275,7 +3289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
         <v>500</v>
       </c>
@@ -3295,7 +3309,7 @@
         <v>20.796457943625501</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="10">
         <v>750</v>
       </c>
@@ -3315,7 +3329,7 @@
         <v>23.7873658351843</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="10">
         <v>1000</v>
       </c>
@@ -3335,7 +3349,7 @@
         <v>32.049815387004898</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="10">
         <v>1500</v>
       </c>
@@ -3355,7 +3369,7 @@
         <v>36.553662630419602</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="10">
         <v>2000</v>
       </c>
@@ -3375,7 +3389,7 @@
         <v>36.199819933617299</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="10">
         <v>2500</v>
       </c>
@@ -3395,7 +3409,7 @@
         <v>34.883576648674499</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="10">
         <v>3000</v>
       </c>
@@ -3415,7 +3429,7 @@
         <v>26.170720170518099</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="10">
         <v>3500</v>
       </c>
@@ -3435,7 +3449,7 @@
         <v>24.0259789996744</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="10">
         <v>4000</v>
       </c>
@@ -3455,7 +3469,7 @@
         <v>17.919262247715199</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="10">
         <v>4500</v>
       </c>
@@ -3475,7 +3489,7 @@
         <v>11.7094069344317</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="10">
         <v>5000</v>
       </c>
@@ -3495,7 +3509,7 @@
         <v>9.5728455338096996</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="10">
         <v>6000</v>
       </c>
@@ -3515,7 +3529,7 @@
         <v>15.9507528838305</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="10">
         <v>7000</v>
       </c>
@@ -3535,7 +3549,7 @@
         <v>18.171129783383801</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="10">
         <v>8000</v>
       </c>
@@ -3555,7 +3569,7 @@
         <v>21.460926597126299</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="10">
         <v>9000</v>
       </c>
@@ -3575,7 +3589,7 @@
         <v>21.8140546213634</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="10">
         <v>10000</v>
       </c>
@@ -3595,7 +3609,7 @@
         <v>21.590511194402801</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="10">
         <v>12500</v>
       </c>
@@ -3615,7 +3629,7 @@
         <v>21.154544192693098</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="10">
         <v>15000</v>
       </c>
@@ -3635,7 +3649,7 @@
         <v>13.3014861114798</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="10">
         <v>17500</v>
       </c>
@@ -3655,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="11">
         <v>20000</v>
       </c>
@@ -3673,6 +3687,12 @@
       </c>
       <c r="F50" s="13">
         <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E51" s="14">
+        <f>MIN(E5:E50)</f>
+        <v>4.7476635514018604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>